<commit_message>
hooked up with local DB
</commit_message>
<xml_diff>
--- a/REST.xlsx
+++ b/REST.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fangzhao/UniProjects/NWEN304/NWEN304Project1Server/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>HTTP Verb</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,22 +191,28 @@
     <t>POST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Defined in server but not used by client</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -232,16 +249,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -268,7 +285,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,7 +376,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C8ECCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -614,24 +631,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.875" style="5"/>
+    <col min="1" max="1" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,8 +668,11 @@
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -668,8 +689,9 @@
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -686,8 +708,9 @@
       <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -704,8 +727,11 @@
       <c r="F4" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -724,8 +750,9 @@
       <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -744,8 +771,9 @@
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -762,134 +790,7 @@
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>